<commit_message>
login form is  done
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>login</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Пароль</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>E-mail</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Пароль</t>
         </is>
       </c>
     </row>
@@ -466,27 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nikita</t>
+          <t>dsa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Petrov</t>
+          <t>sda</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Devidovich</t>
+          <t>asdas</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>demid@gmial.com</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>nekita_1992</t>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>aaa@mail.ru</t>
         </is>
       </c>
     </row>
@@ -496,27 +506,366 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Nikita</t>
+          <t>das</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Petrov</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Devidovich</t>
+          <t>asd</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>demid@gmial.com</t>
+          <t>asda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>nekita_1992</t>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>asda</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>dimass</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>dimass</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>ds</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>dimass</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>dimas</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>dimasik</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sad</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>dimon</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>alex</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>alex</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>alex</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>alex</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>alex</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>alex</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete, change, add v1
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -471,32 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Егор</t>
+          <t>егор</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Губин</t>
+          <t>губин</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Вячеславович</t>
+          <t>выфывфы</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>egor</t>
+          <t>выфв</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Егор</t>
+          <t>выфвыфв</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>egor</t>
+          <t>вфывф</t>
         </is>
       </c>
     </row>
@@ -506,32 +506,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>ddsa</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>dsa</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>fdss</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>fdsfs</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>fdsfds</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>fdsfsf</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Артём</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>Боков</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>выфв</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>выфввыфвф</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>ыфввф</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>выфвф</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete, add, change v2
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,22 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>егор</t>
+          <t>егорdsa2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>губин</t>
+          <t>губин2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>выфывфы</t>
+          <t>выфывфы2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>выфв</t>
+          <t>выфв2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -506,32 +506,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ddsa</t>
+          <t>егор1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dsa</t>
+          <t>губин1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>fdss</t>
+          <t>21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>fdsfs</t>
+          <t>21</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>fdsfds</t>
+          <t>21</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>fdsfsf</t>
+          <t>21</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,137 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Артём</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Боков</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>выфв</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>выфввыфвф</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ыфввф</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>выфвф</t>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>36</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete, add, change v3
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -471,22 +471,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>егорdsa2</t>
+          <t>егорdsa2d</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>губин2</t>
+          <t>губин2d</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>выфывфы2</t>
+          <t>выфывфы2d</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>выфв2</t>
+          <t>выфв2d</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -506,32 +506,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>егор1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>губин1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -541,32 +541,32 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>41</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
     </row>
@@ -576,32 +576,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
     </row>
@@ -611,32 +611,32 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
     </row>
@@ -646,32 +646,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete, add, change v4
</commit_message>
<xml_diff>
--- a/backend/data/users.xlsx
+++ b/backend/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,32 +471,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>егорdsa2d</t>
+          <t>егорdsa2d1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>губин2d</t>
+          <t>губин2d1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>выфывфы2d</t>
+          <t>выфывфы2d1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>выфв2d</t>
+          <t>выфв2d1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>выфвыфв</t>
+          <t>выфвыфв1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>вфывф</t>
+          <t>вфывф1</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>3222</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -576,32 +576,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>36</t>
         </is>
       </c>
     </row>
@@ -611,65 +611,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
-        <is>
-          <t>36</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
         <is>
           <t>3</t>
         </is>

</xml_diff>